<commit_message>
Upload ARMS Nutcomposition_edited document with NA_nutcomp filled in
</commit_message>
<xml_diff>
--- a/NutritionComp/ARMS Nut composition_edited.xlsx
+++ b/NutritionComp/ARMS Nut composition_edited.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmcr\Documents\ARMS_Golden_Git\SW-Madagascar\NutritionComp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkelahan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766C8C86-F896-44A2-BF30-5D63D97103EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB5B5A-DBCC-F247-8C7F-D2D42029E138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{0F6D54AC-2C38-EC4E-8BA4-DF77EF1E39DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25780" windowHeight="13860" xr2:uid="{0F6D54AC-2C38-EC4E-8BA4-DF77EF1E39DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="329">
   <si>
     <t>Can</t>
   </si>
@@ -1483,11 +1483,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C02D22-C5E3-6846-A49B-8DFDD4C89904}">
   <dimension ref="A1:AF159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171:K179"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="2" customWidth="1"/>
@@ -1500,7 +1501,7 @@
     <col min="23" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>317</v>
       </c>
@@ -1576,7 +1577,7 @@
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1604,7 +1605,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1635,7 +1636,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1666,7 +1667,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
     </row>
-    <row r="5" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1704,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
     </row>
-    <row r="6" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1731,7 +1732,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1759,7 +1760,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
     </row>
-    <row r="8" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
@@ -1793,7 +1794,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
     </row>
-    <row r="9" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1827,7 +1828,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1867,7 +1868,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -1895,7 +1896,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
     </row>
-    <row r="12" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -1923,7 +1924,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
     </row>
-    <row r="13" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1951,7 +1952,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1979,7 +1980,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
     </row>
-    <row r="15" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
@@ -2016,7 +2017,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2044,7 +2045,7 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
     </row>
-    <row r="17" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2079,7 +2080,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>10</v>
       </c>
@@ -2110,7 +2111,7 @@
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
     </row>
-    <row r="19" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -2162,7 +2163,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -2211,7 +2212,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
     </row>
-    <row r="21" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -2254,7 +2255,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
     </row>
-    <row r="22" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
@@ -2288,7 +2289,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
     </row>
-    <row r="23" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
@@ -2316,7 +2317,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
     </row>
-    <row r="24" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
@@ -2347,7 +2348,7 @@
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
     </row>
-    <row r="25" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -2381,7 +2382,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
     </row>
-    <row r="26" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>30</v>
       </c>
@@ -2409,7 +2410,7 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
     </row>
-    <row r="27" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
@@ -2436,6 +2437,9 @@
       </c>
       <c r="Q27" s="8">
         <v>41.7</v>
+      </c>
+      <c r="S27" s="6">
+        <v>500</v>
       </c>
       <c r="V27" s="1"/>
       <c r="W27" s="2"/>
@@ -2449,7 +2453,7 @@
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
     </row>
-    <row r="28" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
@@ -2480,7 +2484,7 @@
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
     </row>
-    <row r="29" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>64</v>
       </c>
@@ -2514,7 +2518,7 @@
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
     </row>
-    <row r="30" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>68</v>
       </c>
@@ -2548,7 +2552,7 @@
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
     </row>
-    <row r="31" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>64</v>
       </c>
@@ -2588,7 +2592,7 @@
       <c r="AE31" s="2"/>
       <c r="AF31" s="2"/>
     </row>
-    <row r="32" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>64</v>
       </c>
@@ -2603,6 +2607,9 @@
       </c>
       <c r="E32" s="6">
         <v>156</v>
+      </c>
+      <c r="H32" s="6">
+        <v>448.4</v>
       </c>
       <c r="I32" s="7">
         <v>675</v>
@@ -2619,7 +2626,7 @@
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
     </row>
-    <row r="33" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>73</v>
       </c>
@@ -2650,7 +2657,7 @@
       <c r="AE33" s="2"/>
       <c r="AF33" s="2"/>
     </row>
-    <row r="34" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>68</v>
       </c>
@@ -2669,11 +2676,17 @@
       <c r="F34" s="6">
         <v>156</v>
       </c>
+      <c r="J34" s="6">
+        <v>33</v>
+      </c>
       <c r="L34" s="7">
         <v>232.5</v>
       </c>
       <c r="N34" s="6">
         <v>33</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>15</v>
       </c>
       <c r="R34" s="6">
         <v>5</v>
@@ -2693,7 +2706,7 @@
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
     </row>
-    <row r="35" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>76</v>
       </c>
@@ -2724,7 +2737,7 @@
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
     </row>
-    <row r="36" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>76</v>
       </c>
@@ -2761,7 +2774,7 @@
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
     </row>
-    <row r="37" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>64</v>
       </c>
@@ -2804,7 +2817,7 @@
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
     </row>
-    <row r="38" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>64</v>
       </c>
@@ -2838,7 +2851,7 @@
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
     </row>
-    <row r="39" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
@@ -2866,7 +2879,7 @@
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
     </row>
-    <row r="40" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>64</v>
       </c>
@@ -2900,7 +2913,7 @@
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
     </row>
-    <row r="41" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>30</v>
       </c>
@@ -2931,7 +2944,7 @@
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
     </row>
-    <row r="42" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>73</v>
       </c>
@@ -2965,7 +2978,7 @@
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
     </row>
-    <row r="43" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>73</v>
       </c>
@@ -2996,7 +3009,7 @@
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
     </row>
-    <row r="44" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>30</v>
       </c>
@@ -3027,7 +3040,7 @@
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
     </row>
-    <row r="45" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>64</v>
       </c>
@@ -3073,7 +3086,7 @@
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
     </row>
-    <row r="46" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
@@ -3091,6 +3104,9 @@
       </c>
       <c r="F46" s="6">
         <v>120</v>
+      </c>
+      <c r="H46" s="6">
+        <v>300</v>
       </c>
       <c r="I46" s="6">
         <v>360</v>
@@ -3122,7 +3138,7 @@
       <c r="AE46" s="2"/>
       <c r="AF46" s="2"/>
     </row>
-    <row r="47" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>95</v>
       </c>
@@ -3153,7 +3169,7 @@
       <c r="AE47" s="2"/>
       <c r="AF47" s="2"/>
     </row>
-    <row r="48" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>98</v>
       </c>
@@ -3181,7 +3197,7 @@
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
     </row>
-    <row r="49" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>98</v>
       </c>
@@ -3215,7 +3231,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
     </row>
-    <row r="50" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>98</v>
       </c>
@@ -3246,7 +3262,7 @@
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
     </row>
-    <row r="51" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>98</v>
       </c>
@@ -3274,7 +3290,7 @@
       <c r="AE51" s="2"/>
       <c r="AF51" s="2"/>
     </row>
-    <row r="52" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>98</v>
       </c>
@@ -3305,7 +3321,7 @@
       <c r="AE52" s="2"/>
       <c r="AF52" s="2"/>
     </row>
-    <row r="53" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>98</v>
       </c>
@@ -3333,7 +3349,7 @@
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
     </row>
-    <row r="54" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>73</v>
       </c>
@@ -3367,7 +3383,7 @@
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
     </row>
-    <row r="55" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>73</v>
       </c>
@@ -3407,7 +3423,7 @@
       <c r="AE55" s="2"/>
       <c r="AF55" s="2"/>
     </row>
-    <row r="56" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>73</v>
       </c>
@@ -3438,7 +3454,7 @@
       <c r="AE56" s="2"/>
       <c r="AF56" s="2"/>
     </row>
-    <row r="57" spans="1:32" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:32" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>73</v>
       </c>
@@ -3478,7 +3494,7 @@
       <c r="AE57" s="2"/>
       <c r="AF57" s="2"/>
     </row>
-    <row r="58" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>73</v>
       </c>
@@ -3509,7 +3525,7 @@
       <c r="AE58" s="2"/>
       <c r="AF58" s="2"/>
     </row>
-    <row r="59" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>98</v>
       </c>
@@ -3537,7 +3553,7 @@
       <c r="AE59" s="2"/>
       <c r="AF59" s="2"/>
     </row>
-    <row r="60" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>98</v>
       </c>
@@ -3571,7 +3587,7 @@
       <c r="AE60" s="2"/>
       <c r="AF60" s="2"/>
     </row>
-    <row r="61" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>98</v>
       </c>
@@ -3599,7 +3615,7 @@
       <c r="AE61" s="2"/>
       <c r="AF61" s="2"/>
     </row>
-    <row r="62" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>98</v>
       </c>
@@ -3630,7 +3646,7 @@
       <c r="AE62" s="2"/>
       <c r="AF62" s="2"/>
     </row>
-    <row r="63" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>98</v>
       </c>
@@ -3638,6 +3654,9 @@
         <v>96</v>
       </c>
       <c r="C63" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>126</v>
       </c>
       <c r="E63" s="5">
@@ -3658,7 +3677,7 @@
       <c r="AE63" s="2"/>
       <c r="AF63" s="2"/>
     </row>
-    <row r="64" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>127</v>
       </c>
@@ -3695,7 +3714,7 @@
       <c r="AE64" s="2"/>
       <c r="AF64" s="2"/>
     </row>
-    <row r="65" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
@@ -3726,7 +3745,7 @@
       <c r="AE65" s="2"/>
       <c r="AF65" s="2"/>
     </row>
-    <row r="66" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>127</v>
       </c>
@@ -3754,7 +3773,7 @@
       <c r="AE66" s="2"/>
       <c r="AF66" s="2"/>
     </row>
-    <row r="67" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>127</v>
       </c>
@@ -3782,7 +3801,7 @@
       <c r="AE67" s="2"/>
       <c r="AF67" s="2"/>
     </row>
-    <row r="68" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>127</v>
       </c>
@@ -3810,7 +3829,7 @@
       <c r="AE68" s="2"/>
       <c r="AF68" s="2"/>
     </row>
-    <row r="69" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>127</v>
       </c>
@@ -3838,7 +3857,7 @@
       <c r="AE69" s="2"/>
       <c r="AF69" s="2"/>
     </row>
-    <row r="70" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>127</v>
       </c>
@@ -3853,6 +3872,9 @@
       </c>
       <c r="E70" s="6">
         <v>19</v>
+      </c>
+      <c r="S70" s="7">
+        <v>356.5</v>
       </c>
       <c r="T70" s="6">
         <v>0</v>
@@ -3869,7 +3891,7 @@
       <c r="AE70" s="2"/>
       <c r="AF70" s="2"/>
     </row>
-    <row r="71" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>127</v>
       </c>
@@ -3906,7 +3928,7 @@
       <c r="AE71" s="2"/>
       <c r="AF71" s="2"/>
     </row>
-    <row r="72" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>127</v>
       </c>
@@ -3934,7 +3956,7 @@
       <c r="AE72" s="2"/>
       <c r="AF72" s="2"/>
     </row>
-    <row r="73" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>127</v>
       </c>
@@ -3949,6 +3971,9 @@
       </c>
       <c r="E73" s="6">
         <v>40</v>
+      </c>
+      <c r="H73" s="7">
+        <v>356.5</v>
       </c>
       <c r="L73" s="6">
         <v>180</v>
@@ -3977,7 +4002,7 @@
       <c r="AE73" s="2"/>
       <c r="AF73" s="2"/>
     </row>
-    <row r="74" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>127</v>
       </c>
@@ -4011,7 +4036,7 @@
       <c r="AE74" s="2"/>
       <c r="AF74" s="2"/>
     </row>
-    <row r="75" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>127</v>
       </c>
@@ -4026,6 +4051,9 @@
       </c>
       <c r="E75" s="6">
         <v>58</v>
+      </c>
+      <c r="S75" s="7">
+        <v>356.5</v>
       </c>
       <c r="T75" s="6">
         <v>0</v>
@@ -4042,7 +4070,7 @@
       <c r="AE75" s="2"/>
       <c r="AF75" s="2"/>
     </row>
-    <row r="76" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>127</v>
       </c>
@@ -4082,7 +4110,7 @@
       <c r="AE76" s="2"/>
       <c r="AF76" s="2"/>
     </row>
-    <row r="77" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>127</v>
       </c>
@@ -4110,7 +4138,7 @@
       <c r="AE77" s="2"/>
       <c r="AF77" s="2"/>
     </row>
-    <row r="78" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>127</v>
       </c>
@@ -4138,7 +4166,7 @@
       <c r="AE78" s="2"/>
       <c r="AF78" s="2"/>
     </row>
-    <row r="79" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>127</v>
       </c>
@@ -4169,7 +4197,7 @@
       <c r="AE79" s="2"/>
       <c r="AF79" s="2"/>
     </row>
-    <row r="80" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>76</v>
       </c>
@@ -4206,7 +4234,7 @@
       <c r="AE80" s="2"/>
       <c r="AF80" s="2"/>
     </row>
-    <row r="81" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>162</v>
       </c>
@@ -4237,7 +4265,7 @@
       <c r="AE81" s="2"/>
       <c r="AF81" s="2"/>
     </row>
-    <row r="82" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>162</v>
       </c>
@@ -4268,7 +4296,7 @@
       <c r="AE82" s="2"/>
       <c r="AF82" s="2"/>
     </row>
-    <row r="83" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>76</v>
       </c>
@@ -4308,7 +4336,7 @@
       <c r="AE83" s="2"/>
       <c r="AF83" s="2"/>
     </row>
-    <row r="84" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>76</v>
       </c>
@@ -4336,7 +4364,7 @@
       <c r="AE84" s="2"/>
       <c r="AF84" s="2"/>
     </row>
-    <row r="85" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>171</v>
       </c>
@@ -4351,6 +4379,9 @@
       </c>
       <c r="E85" s="6">
         <v>34</v>
+      </c>
+      <c r="H85" s="7">
+        <v>1360.8</v>
       </c>
       <c r="J85" s="7">
         <v>1360.8</v>
@@ -4367,7 +4398,7 @@
       <c r="AE85" s="2"/>
       <c r="AF85" s="2"/>
     </row>
-    <row r="86" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>76</v>
       </c>
@@ -4398,7 +4429,7 @@
       <c r="AE86" s="2"/>
       <c r="AF86" s="2"/>
     </row>
-    <row r="87" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>171</v>
       </c>
@@ -4426,7 +4457,7 @@
       <c r="AE87" s="2"/>
       <c r="AF87" s="2"/>
     </row>
-    <row r="88" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
@@ -4454,7 +4485,7 @@
       <c r="AE88" s="2"/>
       <c r="AF88" s="2"/>
     </row>
-    <row r="89" spans="1:32" s="5" customFormat="1" ht="30.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>76</v>
       </c>
@@ -4491,7 +4522,7 @@
       <c r="AE89" s="2"/>
       <c r="AF89" s="2"/>
     </row>
-    <row r="90" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
         <v>76</v>
       </c>
@@ -4522,7 +4553,7 @@
       <c r="AE90" s="2"/>
       <c r="AF90" s="2"/>
     </row>
-    <row r="91" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>76</v>
       </c>
@@ -4556,7 +4587,7 @@
       <c r="AE91" s="2"/>
       <c r="AF91" s="2"/>
     </row>
-    <row r="92" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>76</v>
       </c>
@@ -4590,7 +4621,7 @@
       <c r="AE92" s="2"/>
       <c r="AF92" s="2"/>
     </row>
-    <row r="93" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>76</v>
       </c>
@@ -4618,7 +4649,7 @@
       <c r="AE93" s="2"/>
       <c r="AF93" s="2"/>
     </row>
-    <row r="94" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>76</v>
       </c>
@@ -4652,7 +4683,7 @@
       <c r="AE94" s="2"/>
       <c r="AF94" s="2"/>
     </row>
-    <row r="95" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>162</v>
       </c>
@@ -4683,7 +4714,7 @@
       <c r="AE95" s="2"/>
       <c r="AF95" s="2"/>
     </row>
-    <row r="96" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>194</v>
       </c>
@@ -4720,7 +4751,7 @@
       <c r="AE96" s="2"/>
       <c r="AF96" s="2"/>
     </row>
-    <row r="97" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>76</v>
       </c>
@@ -4757,7 +4788,7 @@
       <c r="AE97" s="2"/>
       <c r="AF97" s="2"/>
     </row>
-    <row r="98" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>76</v>
       </c>
@@ -4788,7 +4819,7 @@
       <c r="AE98" s="2"/>
       <c r="AF98" s="2"/>
     </row>
-    <row r="99" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>194</v>
       </c>
@@ -4816,7 +4847,7 @@
       <c r="AE99" s="2"/>
       <c r="AF99" s="2"/>
     </row>
-    <row r="100" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>194</v>
       </c>
@@ -4847,7 +4878,7 @@
       <c r="AE100" s="2"/>
       <c r="AF100" s="2"/>
     </row>
-    <row r="101" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>76</v>
       </c>
@@ -4878,7 +4909,7 @@
       <c r="AE101" s="2"/>
       <c r="AF101" s="2"/>
     </row>
-    <row r="102" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>76</v>
       </c>
@@ -4912,7 +4943,7 @@
       <c r="AE102" s="2"/>
       <c r="AF102" s="2"/>
     </row>
-    <row r="103" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>76</v>
       </c>
@@ -4940,7 +4971,7 @@
       <c r="AE103" s="2"/>
       <c r="AF103" s="2"/>
     </row>
-    <row r="104" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>76</v>
       </c>
@@ -4977,7 +5008,7 @@
       <c r="AE104" s="2"/>
       <c r="AF104" s="2"/>
     </row>
-    <row r="105" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>162</v>
       </c>
@@ -5008,7 +5039,7 @@
       <c r="AE105" s="2"/>
       <c r="AF105" s="2"/>
     </row>
-    <row r="106" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>194</v>
       </c>
@@ -5039,7 +5070,7 @@
       <c r="AE106" s="2"/>
       <c r="AF106" s="2"/>
     </row>
-    <row r="107" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>76</v>
       </c>
@@ -5070,7 +5101,7 @@
       <c r="AE107" s="2"/>
       <c r="AF107" s="2"/>
     </row>
-    <row r="108" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>76</v>
       </c>
@@ -5098,7 +5129,7 @@
       <c r="AE108" s="2"/>
       <c r="AF108" s="2"/>
     </row>
-    <row r="109" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>76</v>
       </c>
@@ -5126,7 +5157,7 @@
       <c r="AE109" s="2"/>
       <c r="AF109" s="2"/>
     </row>
-    <row r="110" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>76</v>
       </c>
@@ -5157,7 +5188,7 @@
       <c r="AE110" s="2"/>
       <c r="AF110" s="2"/>
     </row>
-    <row r="111" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>76</v>
       </c>
@@ -5197,7 +5228,7 @@
       <c r="AE111" s="2"/>
       <c r="AF111" s="2"/>
     </row>
-    <row r="112" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>76</v>
       </c>
@@ -5225,7 +5256,7 @@
       <c r="AE112" s="2"/>
       <c r="AF112" s="2"/>
     </row>
-    <row r="113" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>224</v>
       </c>
@@ -5268,7 +5299,7 @@
       <c r="AE113" s="2"/>
       <c r="AF113" s="2"/>
     </row>
-    <row r="114" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>224</v>
       </c>
@@ -5296,7 +5327,7 @@
       <c r="AE114" s="2"/>
       <c r="AF114" s="2"/>
     </row>
-    <row r="115" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
         <v>224</v>
       </c>
@@ -5333,7 +5364,7 @@
       <c r="AE115" s="2"/>
       <c r="AF115" s="2"/>
     </row>
-    <row r="116" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
         <v>224</v>
       </c>
@@ -5373,7 +5404,7 @@
       <c r="AE116" s="2"/>
       <c r="AF116" s="2"/>
     </row>
-    <row r="117" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
         <v>224</v>
       </c>
@@ -5401,7 +5432,7 @@
       <c r="AE117" s="2"/>
       <c r="AF117" s="2"/>
     </row>
-    <row r="118" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>224</v>
       </c>
@@ -5432,7 +5463,7 @@
       <c r="AE118" s="2"/>
       <c r="AF118" s="2"/>
     </row>
-    <row r="119" spans="1:32" s="13" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
         <v>238</v>
       </c>
@@ -5457,7 +5488,7 @@
       <c r="AE119" s="2"/>
       <c r="AF119" s="2"/>
     </row>
-    <row r="120" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>238</v>
       </c>
@@ -5482,7 +5513,7 @@
       <c r="AE120" s="2"/>
       <c r="AF120" s="2"/>
     </row>
-    <row r="121" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
         <v>238</v>
       </c>
@@ -5507,7 +5538,7 @@
       <c r="AE121" s="2"/>
       <c r="AF121" s="2"/>
     </row>
-    <row r="122" spans="1:32" s="13" customFormat="1" ht="46" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
         <v>246</v>
       </c>
@@ -5535,7 +5566,7 @@
       <c r="AE122" s="2"/>
       <c r="AF122" s="2"/>
     </row>
-    <row r="123" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
         <v>238</v>
       </c>
@@ -5560,7 +5591,7 @@
       <c r="AE123" s="2"/>
       <c r="AF123" s="2"/>
     </row>
-    <row r="124" spans="1:32" s="13" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
         <v>238</v>
       </c>
@@ -5585,7 +5616,7 @@
       <c r="AE124" s="2"/>
       <c r="AF124" s="2"/>
     </row>
-    <row r="125" spans="1:32" s="13" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
         <v>238</v>
       </c>
@@ -5610,7 +5641,7 @@
       <c r="AE125" s="2"/>
       <c r="AF125" s="2"/>
     </row>
-    <row r="126" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>64</v>
       </c>
@@ -5626,10 +5657,16 @@
       <c r="E126" s="6">
         <v>338</v>
       </c>
+      <c r="F126" s="7">
+        <v>124.5</v>
+      </c>
       <c r="G126" s="6">
         <v>360</v>
       </c>
       <c r="J126" s="6">
+        <v>30</v>
+      </c>
+      <c r="O126" s="6">
         <v>30</v>
       </c>
       <c r="V126" s="1"/>
@@ -5644,7 +5681,7 @@
       <c r="AE126" s="2"/>
       <c r="AF126" s="2"/>
     </row>
-    <row r="127" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
         <v>64</v>
       </c>
@@ -5678,7 +5715,7 @@
       <c r="AE127" s="2"/>
       <c r="AF127" s="2"/>
     </row>
-    <row r="128" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
         <v>64</v>
       </c>
@@ -5709,7 +5746,7 @@
       <c r="AE128" s="2"/>
       <c r="AF128" s="2"/>
     </row>
-    <row r="129" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
         <v>76</v>
       </c>
@@ -5740,7 +5777,7 @@
       <c r="AE129" s="2"/>
       <c r="AF129" s="2"/>
     </row>
-    <row r="130" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
         <v>64</v>
       </c>
@@ -5774,7 +5811,7 @@
       <c r="AE130" s="2"/>
       <c r="AF130" s="2"/>
     </row>
-    <row r="131" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>64</v>
       </c>
@@ -5808,7 +5845,7 @@
       <c r="AE131" s="2"/>
       <c r="AF131" s="2"/>
     </row>
-    <row r="132" spans="1:32" s="5" customFormat="1" ht="45.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>64</v>
       </c>
@@ -5851,7 +5888,7 @@
       <c r="AE132" s="2"/>
       <c r="AF132" s="2"/>
     </row>
-    <row r="133" spans="1:32" s="13" customFormat="1" ht="46" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="s">
         <v>326</v>
       </c>
@@ -5876,7 +5913,7 @@
       <c r="AE133" s="2"/>
       <c r="AF133" s="2"/>
     </row>
-    <row r="134" spans="1:32" s="13" customFormat="1" ht="46" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="s">
         <v>326</v>
       </c>
@@ -5901,7 +5938,7 @@
       <c r="AE134" s="2"/>
       <c r="AF134" s="2"/>
     </row>
-    <row r="135" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="6" t="s">
         <v>224</v>
       </c>
@@ -5932,7 +5969,7 @@
       <c r="AE135" s="2"/>
       <c r="AF135" s="2"/>
     </row>
-    <row r="136" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>275</v>
       </c>
@@ -5969,7 +6006,7 @@
       <c r="AE136" s="2"/>
       <c r="AF136" s="2"/>
     </row>
-    <row r="137" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="6" t="s">
         <v>275</v>
       </c>
@@ -6003,7 +6040,7 @@
       <c r="AE137" s="2"/>
       <c r="AF137" s="2"/>
     </row>
-    <row r="138" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="6" t="s">
         <v>275</v>
       </c>
@@ -6031,7 +6068,7 @@
       <c r="AE138" s="2"/>
       <c r="AF138" s="2"/>
     </row>
-    <row r="139" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>281</v>
       </c>
@@ -6065,7 +6102,7 @@
       <c r="AE139" s="2"/>
       <c r="AF139" s="2"/>
     </row>
-    <row r="140" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>284</v>
       </c>
@@ -6099,7 +6136,7 @@
       <c r="AE140" s="2"/>
       <c r="AF140" s="2"/>
     </row>
-    <row r="141" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>15</v>
       </c>
@@ -6142,7 +6179,7 @@
       <c r="AE141" s="2"/>
       <c r="AF141" s="2"/>
     </row>
-    <row r="142" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>15</v>
       </c>
@@ -6163,6 +6200,9 @@
       </c>
       <c r="H142" s="6">
         <v>432.9</v>
+      </c>
+      <c r="J142" s="6">
+        <v>67.400000000000006</v>
       </c>
       <c r="L142" s="8">
         <v>269.60000000000002</v>
@@ -6185,7 +6225,7 @@
       <c r="AE142" s="2"/>
       <c r="AF142" s="2"/>
     </row>
-    <row r="143" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>15</v>
       </c>
@@ -6222,7 +6262,7 @@
       <c r="AE143" s="2"/>
       <c r="AF143" s="2"/>
     </row>
-    <row r="144" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -6271,7 +6311,7 @@
       <c r="AE144" s="2"/>
       <c r="AF144" s="2"/>
     </row>
-    <row r="145" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
         <v>15</v>
       </c>
@@ -6311,7 +6351,7 @@
       <c r="AE145" s="2"/>
       <c r="AF145" s="2"/>
     </row>
-    <row r="146" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:32" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="6" t="s">
         <v>15</v>
       </c>
@@ -6354,7 +6394,7 @@
       <c r="AE146" s="2"/>
       <c r="AF146" s="2"/>
     </row>
-    <row r="147" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="6" t="s">
         <v>15</v>
       </c>
@@ -6394,7 +6434,7 @@
       <c r="AE147" s="2"/>
       <c r="AF147" s="2"/>
     </row>
-    <row r="148" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="6" t="s">
         <v>15</v>
       </c>
@@ -6425,7 +6465,7 @@
       <c r="AE148" s="2"/>
       <c r="AF148" s="2"/>
     </row>
-    <row r="149" spans="1:32" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="6" t="s">
         <v>301</v>
       </c>
@@ -6456,7 +6496,7 @@
       <c r="AE149" s="2"/>
       <c r="AF149" s="2"/>
     </row>
-    <row r="150" spans="1:32" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:32" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A150" s="6" t="s">
         <v>64</v>
       </c>
@@ -6505,7 +6545,7 @@
       <c r="AE150" s="2"/>
       <c r="AF150" s="2"/>
     </row>
-    <row r="151" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:32" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="6" t="s">
         <v>306</v>
       </c>
@@ -6554,7 +6594,7 @@
       <c r="AE151" s="2"/>
       <c r="AF151" s="2"/>
     </row>
-    <row r="152" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
         <v>309</v>
       </c>
@@ -6606,7 +6646,7 @@
       <c r="AE152" s="2"/>
       <c r="AF152" s="2"/>
     </row>
-    <row r="153" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="s">
         <v>224</v>
       </c>
@@ -6637,7 +6677,7 @@
       <c r="AE153" s="2"/>
       <c r="AF153" s="2"/>
     </row>
-    <row r="154" spans="1:32" s="13" customFormat="1" ht="30.7" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="s">
         <v>313</v>
       </c>
@@ -6677,7 +6717,7 @@
       <c r="AE154" s="2"/>
       <c r="AF154" s="2"/>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="P159" s="15"/>
     </row>
   </sheetData>

</xml_diff>